<commit_message>
Se actualizan las librerias para el proyecto
</commit_message>
<xml_diff>
--- a/ReporteEmpleados.xlsx
+++ b/ReporteEmpleados.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>IdEmpleado</t>
   </si>
@@ -32,6 +32,36 @@
     <t>ingresos por empleado</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Enrique</t>
+  </si>
+  <si>
+    <t>Soto</t>
+  </si>
+  <si>
+    <t>Andrade</t>
+  </si>
+  <si>
+    <t>128.0</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>Alfonseca</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>50.0</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -44,7 +74,7 @@
     <t>Montane</t>
   </si>
   <si>
-    <t>652.0</t>
+    <t>25.0</t>
   </si>
   <si>
     <t>3</t>
@@ -59,7 +89,7 @@
     <t>Virgen</t>
   </si>
   <si>
-    <t>404.0</t>
+    <t>16.0</t>
   </si>
 </sst>
 </file>
@@ -134,7 +164,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A6:G8"/>
+  <dimension ref="A6:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" zoomScale="150"/>
   </sheetViews>
@@ -182,7 +212,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>28.0</v>
+        <v>6.0</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
@@ -206,6 +236,46 @@
       </c>
       <c r="F8" s="2" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se corrigen errores y actualizan los reportes de compras, ventas y empleados
</commit_message>
<xml_diff>
--- a/ReporteEmpleados.xlsx
+++ b/ReporteEmpleados.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>IdEmpleado</t>
   </si>
@@ -32,36 +32,6 @@
     <t>ingresos por empleado</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Enrique</t>
-  </si>
-  <si>
-    <t>Soto</t>
-  </si>
-  <si>
-    <t>Andrade</t>
-  </si>
-  <si>
-    <t>128.0</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Aaron</t>
-  </si>
-  <si>
-    <t>Alfonseca</t>
-  </si>
-  <si>
-    <t>Martinez</t>
-  </si>
-  <si>
-    <t>50.0</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -74,22 +44,7 @@
     <t>Montane</t>
   </si>
   <si>
-    <t>25.0</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Erick Raymundo</t>
-  </si>
-  <si>
-    <t>Gonzalez</t>
-  </si>
-  <si>
-    <t>Virgen</t>
-  </si>
-  <si>
-    <t>16.0</t>
+    <t>305.0</t>
   </si>
 </sst>
 </file>
@@ -164,14 +119,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A6:G10"/>
+  <dimension ref="A6:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" zoomScale="150"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="14.81640625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="15.4375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="10.28125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="20.28125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="20.6796875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="16.15234375" customWidth="true" bestFit="true"/>
@@ -212,70 +167,10 @@
         <v>9</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>